<commit_message>
Multiple changes : 1) Module to verify observer name coherence 2) Detecting line break "&#10;" 3) Replace all ";" 4) Make datasets cleaner 5) Changed column position
</commit_message>
<xml_diff>
--- a/data/raw/comptages_terrain/plage/us_med_pnmcca_observatoire_comptage_terrain_plage_2022-08-10.xlsx
+++ b/data/raw/comptages_terrain/plage/us_med_pnmcca_observatoire_comptage_terrain_plage_2022-08-10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="12180" activeTab="2"/>
+    <workbookView windowWidth="27945" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_comptages" sheetId="4" r:id="rId1"/>
@@ -76,8 +76,7 @@
     <t>Arrivée de plusieurs nucs avant le comptage</t>
   </si>
   <si>
-    <t>-bateaux passant dans la zone de baignade
--bateaux dans le chenal non motorisé</t>
+    <t>Bateaux passant dans la zone de baignade. Bateaux dans le chenal non motorisé.</t>
   </si>
 </sst>
 </file>
@@ -769,9 +768,6 @@
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1278,8 +1274,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1346,7 +1342,7 @@
       <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1397,7 +1393,7 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>